<commit_message>
Added another field and fixed SDK version
</commit_message>
<xml_diff>
--- a/cmd/fitgen/internal/profile/sdk/21.94.xlsx
+++ b/cmd/fitgen/internal/profile/sdk/21.94.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96143025-1814-40B7-8663-EF6575C24853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076192A2-40FA-44EA-B99A-CF4F8CDD8F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14107,16 +14107,7 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCC99"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -43890,8 +43881,8 @@
   <dimension ref="A1:P1311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A1188" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C1192" sqref="C1192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43911,7 +43902,7 @@
     <col min="17" max="19" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3570</v>
       </c>
@@ -64293,6 +64284,9 @@
       <c r="I1220" t="s">
         <v>3601</v>
       </c>
+      <c r="P1220" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="1221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1221">

</xml_diff>